<commit_message>
Code with initial tests readys
</commit_message>
<xml_diff>
--- a/rrhh_listado_correos_prueba.xlsx
+++ b/rrhh_listado_correos_prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlospsc/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlospsc/Desktop/envio-correos-comunicado-alexia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{668CC644-F587-8944-B503-766D2100C269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BF4A67-F02D-504C-825E-F6AA80F6FE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1580" windowWidth="28040" windowHeight="17180" xr2:uid="{6E0500E1-C387-B148-8870-DEF50D97257C}"/>
   </bookViews>
@@ -44,22 +44,22 @@
     <t>Correo</t>
   </si>
   <si>
-    <t>Carlos Salinas Real</t>
-  </si>
-  <si>
     <t>Carlos Salinas bewell</t>
   </si>
   <si>
-    <t>Eduardo Reyes bewell</t>
-  </si>
-  <si>
-    <t>cpatricio.scastillo@gmail.com</t>
-  </si>
-  <si>
     <t>csalinas@somosbewell.cl</t>
   </si>
   <si>
-    <t>eduardo.reyes@somosbewell.cl</t>
+    <t>Claudio Cáceres</t>
+  </si>
+  <si>
+    <t>ccaceres@somosbewell.cl</t>
+  </si>
+  <si>
+    <t>Katherinne Campos</t>
+  </si>
+  <si>
+    <t>katherinne.campos@somosbewell.cl</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,20 +463,20 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -484,9 +484,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{77F35EF6-0192-5F47-8A86-F7CCC5313339}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{7915666C-01B6-D74C-931B-11446ED7D428}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{1981C57B-E3E7-E545-B418-DAFB4BC1854E}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7915666C-01B6-D74C-931B-11446ED7D428}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{9DC9C359-B704-2343-9610-1E2737B3A09C}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{7E599718-43CA-7F42-B769-45F2D8F308D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>